<commit_message>
adding references to spreadsheet
</commit_message>
<xml_diff>
--- a/data/data-sources.xlsx
+++ b/data/data-sources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="900" windowWidth="21495" windowHeight="8610"/>
+    <workbookView xWindow="510" yWindow="900" windowWidth="18345" windowHeight="4095"/>
   </bookViews>
   <sheets>
     <sheet name="data sources" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="514">
   <si>
     <t>http://www.gbif.org/</t>
   </si>
@@ -794,6 +794,777 @@
   <si>
     <t>Our program is intensive and hands-on. Fellows work with nonprofits, local governments, and federal agencies, learning about what they do and tackling data problems they face.
 We believe in open knowledge and open source. We blog extensively about our projects, and make much of our research and code open to everyone.</t>
+  </si>
+  <si>
+    <t>A Guide to Actionable Measurement</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=166</t>
+  </si>
+  <si>
+    <t>Bill &amp; Melinda Gates Foundation</t>
+  </si>
+  <si>
+    <t>Best Practice</t>
+  </si>
+  <si>
+    <t>A Practical Guide for Engaging Stakeholders in Developing Evaluation Questions</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=152</t>
+  </si>
+  <si>
+    <t>FSG</t>
+  </si>
+  <si>
+    <t>Alliance for Justice Advocacy Capacity Tool (ACT)</t>
+  </si>
+  <si>
+    <t>Bolder Advocacy project of Alliance for Justice</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=8</t>
+  </si>
+  <si>
+    <t>Application Perception Report (APR)</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=37</t>
+  </si>
+  <si>
+    <t>Center for Effective Philanthropy</t>
+  </si>
+  <si>
+    <t>Appreciative Inquiry Approach</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=9</t>
+  </si>
+  <si>
+    <t>Annie E. Casey Foundation, Organizational Research Services</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Apricot Outcomes Achievement Software</t>
+  </si>
+  <si>
+    <t>Community TechKnowledge</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=180</t>
+  </si>
+  <si>
+    <t>Ashoka Measuring Effectiveness Questionnaire</t>
+  </si>
+  <si>
+    <t>Ashoka</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=27</t>
+  </si>
+  <si>
+    <t>Assessing and Building Your Organization's Capacity</t>
+  </si>
+  <si>
+    <t>Capable Partners Program (CAP), NGO Connect</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=190</t>
+  </si>
+  <si>
+    <t>Assessing Number and Type of Policies</t>
+  </si>
+  <si>
+    <t>Assessment and Improvement Indicators</t>
+  </si>
+  <si>
+    <t>Venture Philanthropy Partners</t>
+  </si>
+  <si>
+    <t>BACO Ratio</t>
+  </si>
+  <si>
+    <t>Acumen Fund</t>
+  </si>
+  <si>
+    <t>Balanced Scorecard</t>
+  </si>
+  <si>
+    <t>New Profit, Inc.</t>
+  </si>
+  <si>
+    <t>Base of Pyramid Impact Assessment Framework</t>
+  </si>
+  <si>
+    <t>William Davidson Institute</t>
+  </si>
+  <si>
+    <t>BBB Wise Giving Alliance Seal</t>
+  </si>
+  <si>
+    <t>Better Business Bureau</t>
+  </si>
+  <si>
+    <t>certified</t>
+  </si>
+  <si>
+    <t>Beneficiary Perception Report (BPR)</t>
+  </si>
+  <si>
+    <t>Benefit-Cost Analysis</t>
+  </si>
+  <si>
+    <t>Abt Associates</t>
+  </si>
+  <si>
+    <t>Benefit-Cost Ratio</t>
+  </si>
+  <si>
+    <t>Robin Hood Foundation</t>
+  </si>
+  <si>
+    <t>Billboard Survey Form</t>
+  </si>
+  <si>
+    <t>Annie E. Casey Foundation, FACE</t>
+  </si>
+  <si>
+    <t>BluePrint 1.0</t>
+  </si>
+  <si>
+    <t>Blue Ridge Foundation</t>
+  </si>
+  <si>
+    <t>Board Service ROI Tracker</t>
+  </si>
+  <si>
+    <t>True Impact (with Points of Light/HandsOn Network)</t>
+  </si>
+  <si>
+    <t>Born Learning Washington Monthly Media Tracking Form</t>
+  </si>
+  <si>
+    <t>Build Initiative Checklist</t>
+  </si>
+  <si>
+    <t>Annie E. Casey Foundation, Build, Organizational Research Services</t>
+  </si>
+  <si>
+    <t>http://unstats.un.org/unsd/demographic/products/socind/</t>
+  </si>
+  <si>
+    <t>Social indicators</t>
+  </si>
+  <si>
+    <t>http://35.8.121.111/si/home.aspx</t>
+  </si>
+  <si>
+    <t>Using Social Indicators for Evaluating Nonpoint Source (NPS) Management Efforts</t>
+  </si>
+  <si>
+    <t>http://www.oecd.org/social/soc/</t>
+  </si>
+  <si>
+    <t>Social policies and data</t>
+  </si>
+  <si>
+    <t>http://www.ciesin.org/IC/wbank/sid-home.html</t>
+  </si>
+  <si>
+    <t>Social Indicators of Development</t>
+  </si>
+  <si>
+    <t>Building a Performance Measurement System</t>
+  </si>
+  <si>
+    <t>Building Future Leaders Diagnostic Survey</t>
+  </si>
+  <si>
+    <t>Campaign Champions Data Collection Tool</t>
+  </si>
+  <si>
+    <t>Capabilities Profiler</t>
+  </si>
+  <si>
+    <t>Changes in Attitudes Focus Group</t>
+  </si>
+  <si>
+    <t>Charity Analysis Framework</t>
+  </si>
+  <si>
+    <t>Charity Navigator Rating</t>
+  </si>
+  <si>
+    <t>Charting Impact</t>
+  </si>
+  <si>
+    <t>Checklist for Reviewing a Randomized Controlled Trial or a Social Program or Project</t>
+  </si>
+  <si>
+    <t>Civic Engagement Measurement System (CEMS)</t>
+  </si>
+  <si>
+    <t>Cluster Evaluation</t>
+  </si>
+  <si>
+    <t>Community Health Assessment aNd Group Evaluation (CHANGE)</t>
+  </si>
+  <si>
+    <t>Community Members' Perceptions about Prioritization of Issues Survey</t>
+  </si>
+  <si>
+    <t>Community of Learners</t>
+  </si>
+  <si>
+    <t>Community Tool Box</t>
+  </si>
+  <si>
+    <t>Comparative Constituency Feedback</t>
+  </si>
+  <si>
+    <t>Compass Index Sustainability Assessment</t>
+  </si>
+  <si>
+    <t>Considering Evaluation</t>
+  </si>
+  <si>
+    <t>Core Capacity Assessment Tool (CCAT)</t>
+  </si>
+  <si>
+    <t>Cost Benefit Analysis</t>
+  </si>
+  <si>
+    <t>Cost Effectiveness Analysis</t>
+  </si>
+  <si>
+    <t>Cost per Impact</t>
+  </si>
+  <si>
+    <t>Cradle to Cradle Certification</t>
+  </si>
+  <si>
+    <t>Criteria for Philanthropy at Its Best</t>
+  </si>
+  <si>
+    <t>Cultural Data Project</t>
+  </si>
+  <si>
+    <t>Dalberg Approach</t>
+  </si>
+  <si>
+    <t>Developing a Theory of Change</t>
+  </si>
+  <si>
+    <t>Development Outcome Tracking System (DOTS)</t>
+  </si>
+  <si>
+    <t>DevResults</t>
+  </si>
+  <si>
+    <t>Donor Committee for Enterprise Development (DCED) Standard</t>
+  </si>
+  <si>
+    <t>Donor Perception Report (DPR)</t>
+  </si>
+  <si>
+    <t>Due Diligence Framework for Scaling Initiatives</t>
+  </si>
+  <si>
+    <t>Echoing Green Mid-Year and Year End Reports</t>
+  </si>
+  <si>
+    <t>Ecological Footprint</t>
+  </si>
+  <si>
+    <t>Efforts to Outcomes (ETO) Software</t>
+  </si>
+  <si>
+    <t>Environmental Performance Reporting System (EPRS)</t>
+  </si>
+  <si>
+    <t>Evaluating Development Co-Operation</t>
+  </si>
+  <si>
+    <t>Evaluating the Impact of Development Projects on Poverty: A Handbook for Practitioners</t>
+  </si>
+  <si>
+    <t>Evaluation Plan Builder</t>
+  </si>
+  <si>
+    <t>Evaluation Principles and Practices</t>
+  </si>
+  <si>
+    <t>Excellence Model</t>
+  </si>
+  <si>
+    <t>Expected Return</t>
+  </si>
+  <si>
+    <t>External Review of Program Strategy (Getting an Expert View)</t>
+  </si>
+  <si>
+    <t>Fair Trade Certification</t>
+  </si>
+  <si>
+    <t>Foundation Performance Assessment Framework</t>
+  </si>
+  <si>
+    <t>Foundation Scorecard</t>
+  </si>
+  <si>
+    <t>Foundations of Success Guideline for Effective Evaluation</t>
+  </si>
+  <si>
+    <t>Framework for Program Evaluation</t>
+  </si>
+  <si>
+    <t>Gender Equality Principles Initiative</t>
+  </si>
+  <si>
+    <t>Getting to Outcomes™</t>
+  </si>
+  <si>
+    <t>GIRAFE</t>
+  </si>
+  <si>
+    <t>GiveWell Method</t>
+  </si>
+  <si>
+    <t>Global Impact Investing Ratings System</t>
+  </si>
+  <si>
+    <t>Grantee Perception Report (GPR)</t>
+  </si>
+  <si>
+    <t>GreatNonprofits Reviews</t>
+  </si>
+  <si>
+    <t>GRI Reporting Framework</t>
+  </si>
+  <si>
+    <t>GuideStar Analyst Reports</t>
+  </si>
+  <si>
+    <t>HAP Humanitarian Accountability and Quality Management Standard</t>
+  </si>
+  <si>
+    <t>HIP (Human Impact + Profit) Scorecard ™</t>
+  </si>
+  <si>
+    <t>Impact Framework</t>
+  </si>
+  <si>
+    <t>Impact Reporting and Investment Standards (IRIS)</t>
+  </si>
+  <si>
+    <t>Intensity of Integration Tracking Form</t>
+  </si>
+  <si>
+    <t>Interrupted Time Series Designs</t>
+  </si>
+  <si>
+    <t>KaBOOM! Method</t>
+  </si>
+  <si>
+    <t>KIDS COUNT Media Tracking Form</t>
+  </si>
+  <si>
+    <t>KIDS COUNT Self-Assessment Tool</t>
+  </si>
+  <si>
+    <t>LBG Measuring and Benchmarking Corportate Community Investment</t>
+  </si>
+  <si>
+    <t>Leadership in Energy and Environmental Design Certification (LEED)</t>
+  </si>
+  <si>
+    <t>Learning for Results</t>
+  </si>
+  <si>
+    <t>Learning with Constituents</t>
+  </si>
+  <si>
+    <t>Legislative Process Tracking Log</t>
+  </si>
+  <si>
+    <t>Listen First Framework</t>
+  </si>
+  <si>
+    <t>Listen Learn Lead</t>
+  </si>
+  <si>
+    <t>Local Multiplier 3</t>
+  </si>
+  <si>
+    <t>Logic Model Builder</t>
+  </si>
+  <si>
+    <t>Making the Case™</t>
+  </si>
+  <si>
+    <t>Measurement of Cultural Vitality</t>
+  </si>
+  <si>
+    <t>Measures of Success</t>
+  </si>
+  <si>
+    <t>Measuring Advocacy and Policy</t>
+  </si>
+  <si>
+    <t>Measuring Impact Framework</t>
+  </si>
+  <si>
+    <t>Meeting Observation Checklist</t>
+  </si>
+  <si>
+    <t>Methodology for Impact Analysis and Assessment (MIAA)</t>
+  </si>
+  <si>
+    <t>Metrics Guide</t>
+  </si>
+  <si>
+    <t>Metrics that Matter</t>
+  </si>
+  <si>
+    <t>MicroRate</t>
+  </si>
+  <si>
+    <t>Monitoring &amp; Evaluation Toolkit</t>
+  </si>
+  <si>
+    <t>Monitoring and Evaluation for Poverty Reduction</t>
+  </si>
+  <si>
+    <t>Movement Above the U.S. $1 a Day Threshold</t>
+  </si>
+  <si>
+    <t>Multidimensional Assessment Process (MAP)</t>
+  </si>
+  <si>
+    <t>Nurse-Family Partnership Evaluation &amp; Logic Models</t>
+  </si>
+  <si>
+    <t>Operational Benchmarking Report (OBR)</t>
+  </si>
+  <si>
+    <t>Organizational Assessment Tool</t>
+  </si>
+  <si>
+    <t>Organizational Capacity Assessment Tool</t>
+  </si>
+  <si>
+    <t>Organizational Capacity Assessment Tool (OCAT)</t>
+  </si>
+  <si>
+    <t>Outcome Mapping</t>
+  </si>
+  <si>
+    <t>Outcome-Based Evaluation</t>
+  </si>
+  <si>
+    <t>Outcomes and Impact Frameworks</t>
+  </si>
+  <si>
+    <t>PCV Social Impact Assessment</t>
+  </si>
+  <si>
+    <t>Performance Information that Really Performs</t>
+  </si>
+  <si>
+    <t>PerformWell</t>
+  </si>
+  <si>
+    <t>Philanthropedia</t>
+  </si>
+  <si>
+    <t>Policy Brief Stakeholder Survey</t>
+  </si>
+  <si>
+    <t>Policy Tracking Analysis Tool</t>
+  </si>
+  <si>
+    <t>Policy Tracking Form</t>
+  </si>
+  <si>
+    <t>Political Return on Investment (PROI)</t>
+  </si>
+  <si>
+    <t>Poverty and Social Impact Analysis (PSIA)</t>
+  </si>
+  <si>
+    <t>PQASSO</t>
+  </si>
+  <si>
+    <t>Pro Bono Manager</t>
+  </si>
+  <si>
+    <t>Program and Policymaking Evaluation</t>
+  </si>
+  <si>
+    <t>Programme Accountability and Learning System (PALS)</t>
+  </si>
+  <si>
+    <t>Progress out of Poverty Index (PPI)</t>
+  </si>
+  <si>
+    <t>Project Level Evaluation: Context Evaluation</t>
+  </si>
+  <si>
+    <t>Project Level Evaluation: Implementation Evaluation</t>
+  </si>
+  <si>
+    <t>Project Level Evaluation: Outcome Evaluation</t>
+  </si>
+  <si>
+    <t>Project Streamline Grantmaker Assessment Tool</t>
+  </si>
+  <si>
+    <t>Prove It!</t>
+  </si>
+  <si>
+    <t>Pulse</t>
+  </si>
+  <si>
+    <t>Quality Audit Tool for Managing Performance (QAT)</t>
+  </si>
+  <si>
+    <t>Quality of Official Development Assistance (QuODA) Assessment</t>
+  </si>
+  <si>
+    <t>Roca’s High-Risk Youth Intervention Model</t>
+  </si>
+  <si>
+    <t>SEEP Client Exit Survey</t>
+  </si>
+  <si>
+    <t>SEEP Client Satisfaction Focus Group</t>
+  </si>
+  <si>
+    <t>SEEP Empowerment Interview</t>
+  </si>
+  <si>
+    <t>SEEP Impact Survey</t>
+  </si>
+  <si>
+    <t>SEEP Loan and Savings Use Interview</t>
+  </si>
+  <si>
+    <t>SOCIAL</t>
+  </si>
+  <si>
+    <t>Social Audit</t>
+  </si>
+  <si>
+    <t>Social e-valuator</t>
+  </si>
+  <si>
+    <t>Social Impact Assessment</t>
+  </si>
+  <si>
+    <t>Social Impact Assessment (SIA)</t>
+  </si>
+  <si>
+    <t>Social IMPact Measurement for Local Economies (SIMPLE)</t>
+  </si>
+  <si>
+    <t>Social Impact Tracker</t>
+  </si>
+  <si>
+    <t>Social Investment Risk Assessment (SIRA)</t>
+  </si>
+  <si>
+    <t>Social Outcome Tracking</t>
+  </si>
+  <si>
+    <t>Social Performance Audit Tool</t>
+  </si>
+  <si>
+    <t>Social Performance Indicators (SPI)</t>
+  </si>
+  <si>
+    <t>Social Rating</t>
+  </si>
+  <si>
+    <t>Social Value Metrics</t>
+  </si>
+  <si>
+    <t>SPEAK (Strategic Planning, Evaluation and Knowledge Networking)</t>
+  </si>
+  <si>
+    <t>Spider Diagram for Capacity Building Advocacy</t>
+  </si>
+  <si>
+    <t>SROI</t>
+  </si>
+  <si>
+    <t>SROI Framework</t>
+  </si>
+  <si>
+    <t>SROI Lite</t>
+  </si>
+  <si>
+    <t>SROI Toolkit</t>
+  </si>
+  <si>
+    <t>Staff Perception Report (SPR)</t>
+  </si>
+  <si>
+    <t>Stakeholder Assessment Report (STAR)</t>
+  </si>
+  <si>
+    <t>Standards for Excellence® Program</t>
+  </si>
+  <si>
+    <t>Steps Program Evaluation</t>
+  </si>
+  <si>
+    <t>STEPS Toolkit</t>
+  </si>
+  <si>
+    <t>Success Measures Data System (SMDS)</t>
+  </si>
+  <si>
+    <t>Survey of Constituents Receiving "Issue Alerts"</t>
+  </si>
+  <si>
+    <t>TBL Scorecard</t>
+  </si>
+  <si>
+    <t>The B Impact Ratings System</t>
+  </si>
+  <si>
+    <t>The Big Picture</t>
+  </si>
+  <si>
+    <t>The Due Dilligence Tool</t>
+  </si>
+  <si>
+    <t>The FINCA Client Assessment Tool (FCAT)</t>
+  </si>
+  <si>
+    <t>The Harvard Analytical Framework</t>
+  </si>
+  <si>
+    <t>The Outcomes Star</t>
+  </si>
+  <si>
+    <t>The Readiness for Organizational Learning and Evaluation (ROLE) Instrument</t>
+  </si>
+  <si>
+    <t>The Shujog Impact Framework and Assessment</t>
+  </si>
+  <si>
+    <t>Theories of Change</t>
+  </si>
+  <si>
+    <t>Theory of Change Community</t>
+  </si>
+  <si>
+    <t>Trucost</t>
+  </si>
+  <si>
+    <t>Trustee Evaluation Toolkit</t>
+  </si>
+  <si>
+    <t>Understanding Software for Program Evaluation</t>
+  </si>
+  <si>
+    <t>Volunteering Impact Assessment Toolkit</t>
+  </si>
+  <si>
+    <t>Volunteerism ROI Tracker</t>
+  </si>
+  <si>
+    <t>Wallace Assessment Tool</t>
+  </si>
+  <si>
+    <t>Women's Empowerment Framework</t>
+  </si>
+  <si>
+    <t>Root Cause</t>
+  </si>
+  <si>
+    <t>The Bridgespan Group</t>
+  </si>
+  <si>
+    <t>Keystone Accountability</t>
+  </si>
+  <si>
+    <t>New Philanthropy Capital</t>
+  </si>
+  <si>
+    <t>Charity Navigator</t>
+  </si>
+  <si>
+    <t>Independent Sector, BBB Wise Giving Alliance and GuideStar USA</t>
+  </si>
+  <si>
+    <t>Coalition for Evidence-Based Policy</t>
+  </si>
+  <si>
+    <t>The Alliance for Children and Families</t>
+  </si>
+  <si>
+    <t>W.K. Kellogg Foundation</t>
+  </si>
+  <si>
+    <t>Centers for Disease Control and Prevention</t>
+  </si>
+  <si>
+    <t>TCC Group</t>
+  </si>
+  <si>
+    <t>Work Group for Community Health and Development at the University of Kansas</t>
+  </si>
+  <si>
+    <t>AtKisson, Inc.</t>
+  </si>
+  <si>
+    <t>ActKnowledge</t>
+  </si>
+  <si>
+    <t>Center for High Impact Philanthropy</t>
+  </si>
+  <si>
+    <t>Cradle to Cradle</t>
+  </si>
+  <si>
+    <t>National Committee for Responsive Philanthropy</t>
+  </si>
+  <si>
+    <t>The Pew Charitable Trusts</t>
+  </si>
+  <si>
+    <t>Dalberg Global Development Advisors</t>
+  </si>
+  <si>
+    <t>International Finance Corporation (IFC)</t>
+  </si>
+  <si>
+    <t>CaudillWeb</t>
+  </si>
+  <si>
+    <t>The Donor Committee for Enterprise Development</t>
+  </si>
+  <si>
+    <t>Social Impact Exchange, Alliance for Social Investment</t>
+  </si>
+  <si>
+    <t>Echoing Green</t>
+  </si>
+  <si>
+    <t>Global Footprint Network</t>
+  </si>
+  <si>
+    <t>Social Solutions</t>
+  </si>
+  <si>
+    <t>tools and resources for assessing social impact</t>
   </si>
 </sst>
 </file>
@@ -820,7 +1591,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -830,6 +1601,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -846,7 +1623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -863,12 +1640,20 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1164,10 +1949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U102"/>
+  <dimension ref="B1:U302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2620,7 +3405,7 @@
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
     </row>
-    <row r="54" spans="2:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:21" ht="60" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>133</v>
       </c>
@@ -3888,10 +4673,14 @@
       <c r="T100" s="1"/>
       <c r="U100" s="1"/>
     </row>
-    <row r="101" spans="2:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B101" s="1"/>
+    <row r="101" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="B101" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
+      <c r="D101" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
@@ -3910,15 +4699,1648 @@
       <c r="T101" s="1"/>
       <c r="U101" s="1"/>
     </row>
-    <row r="102" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="2" t="s">
+    <row r="102" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1"/>
+      <c r="T102" s="1"/>
+      <c r="U102" s="1"/>
+    </row>
+    <row r="103" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="B103" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+      <c r="R103" s="1"/>
+      <c r="S103" s="1"/>
+      <c r="T103" s="1"/>
+      <c r="U103" s="1"/>
+    </row>
+    <row r="104" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="B104" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+      <c r="R104" s="1"/>
+      <c r="S104" s="1"/>
+      <c r="T104" s="1"/>
+      <c r="U104" s="1"/>
+    </row>
+    <row r="105" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="1"/>
+      <c r="S105" s="1"/>
+      <c r="T105" s="1"/>
+      <c r="U105" s="1"/>
+    </row>
+    <row r="106" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>256</v>
+      </c>
+    </row>
+    <row r="108" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="110" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="111" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="112" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="6"/>
+      <c r="C118" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="6"/>
+      <c r="C119" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="6"/>
+      <c r="C120" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="6"/>
+      <c r="C121" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="6"/>
+      <c r="C122" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="6"/>
+      <c r="C123" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="6"/>
+      <c r="C124" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="6"/>
+      <c r="C125" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="6"/>
+      <c r="C126" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="6"/>
+      <c r="C127" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="6"/>
+      <c r="C128" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="6"/>
+      <c r="C129" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="6"/>
+      <c r="C130" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="6"/>
+      <c r="C131" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="6"/>
+      <c r="C132" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="6"/>
+      <c r="C133" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="6"/>
+      <c r="C134" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="6"/>
+      <c r="C135" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="6"/>
+      <c r="C136" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="6"/>
+      <c r="C137" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="6"/>
+      <c r="C138" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="6"/>
+      <c r="C139" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="6"/>
+      <c r="C140" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="141" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="6"/>
+      <c r="C141" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="142" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="6"/>
+      <c r="C142" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="143" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="6"/>
+      <c r="C143" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="144" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="6"/>
+      <c r="C144" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="6"/>
+      <c r="C145" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="146" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="6"/>
+      <c r="C146" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="6"/>
+      <c r="C147" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="6"/>
+      <c r="C148" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G148" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="6"/>
+      <c r="C149" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B150" s="6"/>
+      <c r="C150" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="151" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="6"/>
+      <c r="C151" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="152" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="6"/>
+      <c r="C152" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="153" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="6"/>
+      <c r="C153" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B154" s="6"/>
+      <c r="C154" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G154" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="6"/>
+      <c r="C155" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="156" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="6"/>
+      <c r="C156" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="157" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="6"/>
+      <c r="C157" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="6"/>
+      <c r="C158" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="6"/>
+      <c r="C159" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="160" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="6"/>
+      <c r="C160" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="6"/>
+      <c r="C161" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="6"/>
+      <c r="C162" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="6"/>
+      <c r="C163" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="6"/>
+      <c r="C164" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="6"/>
+      <c r="C165" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="F165" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G165" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="6"/>
+      <c r="C166" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="F166" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="167" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="6"/>
+      <c r="C167" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="6"/>
+      <c r="C168" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B169" s="6"/>
+      <c r="C169" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B170" s="6"/>
+      <c r="C170" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="171" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B171" s="6"/>
+      <c r="C171" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B172" s="6"/>
+      <c r="C172" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B173" s="6"/>
+      <c r="C173" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B174" s="6"/>
+      <c r="C174" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B175" s="6"/>
+      <c r="C175" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="176" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B176" s="6"/>
+      <c r="C176" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B177" s="6"/>
+      <c r="C177" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="178" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B178" s="6"/>
+      <c r="C178" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="179" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="6"/>
+      <c r="C179" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="180" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B180" s="6"/>
+      <c r="C180" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="181" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B181" s="6"/>
+      <c r="C181" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="182" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B182" s="6"/>
+      <c r="C182" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="183" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B183" s="6"/>
+      <c r="C183" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="184" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B184" s="6"/>
+      <c r="C184" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="185" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B185" s="6"/>
+      <c r="C185" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="186" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B186" s="6"/>
+      <c r="C186" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="187" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B187" s="6"/>
+      <c r="C187" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="188" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B188" s="6"/>
+      <c r="C188" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="189" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B189" s="6"/>
+      <c r="C189" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="190" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B190" s="6"/>
+      <c r="C190" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="191" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B191" s="6"/>
+      <c r="C191" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="192" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B192" s="6"/>
+      <c r="C192" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B193" s="6"/>
+      <c r="C193" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="194" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B194" s="6"/>
+      <c r="C194" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="195" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B195" s="6"/>
+      <c r="C195" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="196" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B196" s="6"/>
+      <c r="C196" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="197" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B197" s="6"/>
+      <c r="C197" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B198" s="6"/>
+      <c r="C198" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="199" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B199" s="6"/>
+      <c r="C199" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B200" s="6"/>
+      <c r="C200" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="201" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B201" s="6"/>
+      <c r="C201" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="202" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B202" s="6"/>
+      <c r="C202" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="203" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B203" s="6"/>
+      <c r="C203" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="204" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B204" s="6"/>
+      <c r="C204" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="205" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B205" s="6"/>
+      <c r="C205" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="206" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B206" s="6"/>
+      <c r="C206" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="207" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B207" s="6"/>
+      <c r="C207" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="208" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B208" s="6"/>
+      <c r="C208" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B209" s="6"/>
+      <c r="C209" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B210" s="6"/>
+      <c r="C210" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B211" s="6"/>
+      <c r="C211" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B212" s="6"/>
+      <c r="C212" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B213" s="6"/>
+      <c r="C213" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="214" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B214" s="6"/>
+      <c r="C214" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B215" s="6"/>
+      <c r="C215" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="216" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B216" s="6"/>
+      <c r="C216" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B217" s="6"/>
+      <c r="C217" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B218" s="6"/>
+      <c r="C218" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B219" s="6"/>
+      <c r="C219" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="220" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B220" s="6"/>
+      <c r="C220" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="221" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B221" s="6"/>
+      <c r="C221" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="222" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B222" s="6"/>
+      <c r="C222" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="223" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B223" s="6"/>
+      <c r="C223" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="224" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B224" s="6"/>
+      <c r="C224" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="225" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B225" s="6"/>
+      <c r="C225" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="226" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B226" s="6"/>
+      <c r="C226" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="227" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B227" s="6"/>
+      <c r="C227" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="228" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B228" s="6"/>
+      <c r="C228" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="229" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B229" s="6"/>
+      <c r="C229" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="230" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B230" s="6"/>
+      <c r="C230" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="231" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B231" s="6"/>
+      <c r="C231" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="232" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B232" s="6"/>
+      <c r="C232" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="233" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B233" s="6"/>
+      <c r="C233" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="234" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B234" s="6"/>
+      <c r="C234" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="235" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B235" s="6"/>
+      <c r="C235" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="236" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B236" s="6"/>
+      <c r="C236" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="237" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B237" s="6"/>
+      <c r="C237" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="238" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B238" s="6"/>
+      <c r="C238" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="239" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B239" s="6"/>
+      <c r="C239" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="240" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B240" s="6"/>
+      <c r="C240" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="241" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B241" s="6"/>
+      <c r="C241" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="242" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B242" s="6"/>
+      <c r="C242" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="243" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B243" s="6"/>
+      <c r="C243" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="244" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B244" s="6"/>
+      <c r="C244" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="245" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B245" s="6"/>
+      <c r="C245" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="246" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B246" s="6"/>
+      <c r="C246" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="247" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B247" s="6"/>
+      <c r="C247" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="248" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B248" s="6"/>
+      <c r="C248" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="249" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B249" s="6"/>
+      <c r="C249" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="250" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B250" s="6"/>
+      <c r="C250" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="251" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B251" s="6"/>
+      <c r="C251" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="252" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B252" s="6"/>
+      <c r="C252" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="253" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B253" s="6"/>
+      <c r="C253" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="254" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B254" s="6"/>
+      <c r="C254" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="255" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B255" s="6"/>
+      <c r="C255" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="256" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B256" s="6"/>
+      <c r="C256" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="257" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B257" s="6"/>
+      <c r="C257" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="258" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B258" s="6"/>
+      <c r="C258" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="259" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B259" s="6"/>
+      <c r="C259" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="260" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B260" s="6"/>
+      <c r="C260" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="261" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B261" s="6"/>
+      <c r="C261" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="262" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B262" s="6"/>
+      <c r="C262" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="263" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B263" s="6"/>
+      <c r="C263" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="264" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B264" s="6"/>
+      <c r="C264" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="265" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B265" s="6"/>
+      <c r="C265" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="266" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B266" s="6"/>
+      <c r="C266" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="267" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B267" s="6"/>
+      <c r="C267" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="268" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B268" s="6"/>
+      <c r="C268" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="269" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B269" s="6"/>
+      <c r="C269" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="270" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B270" s="6"/>
+      <c r="C270" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="271" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B271" s="6"/>
+      <c r="C271" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="272" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B272" s="6"/>
+      <c r="C272" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="273" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B273" s="6"/>
+      <c r="C273" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="274" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B274" s="6"/>
+      <c r="C274" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="275" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B275" s="6"/>
+      <c r="C275" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="276" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B276" s="6"/>
+      <c r="C276" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="277" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B277" s="6"/>
+      <c r="C277" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="278" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B278" s="6"/>
+      <c r="C278" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="279" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B279" s="6"/>
+      <c r="C279" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="280" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B280" s="6"/>
+      <c r="C280" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="281" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B281" s="6"/>
+      <c r="C281" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="282" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B282" s="6"/>
+      <c r="C282" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="283" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B283" s="6"/>
+      <c r="C283" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="284" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B284" s="6"/>
+      <c r="C284" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="285" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B285" s="6"/>
+      <c r="C285" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="286" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B286" s="6"/>
+      <c r="C286" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="287" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B287" s="6"/>
+      <c r="C287" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="288" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B288" s="6"/>
+      <c r="C288" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="289" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B289" s="6"/>
+      <c r="C289" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="290" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B290" s="6"/>
+      <c r="C290" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="291" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B291" s="6"/>
+      <c r="C291" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="292" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B292" s="6"/>
+      <c r="C292" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="293" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B293" s="6"/>
+      <c r="C293" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="294" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B294" s="6"/>
+      <c r="C294" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="295" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B295" s="6"/>
+      <c r="C295" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="296" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B296" s="6"/>
+      <c r="C296" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="297" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B297" s="6"/>
+      <c r="C297" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="298" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B298" s="6"/>
+      <c r="C298" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="299" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B299" s="6"/>
+      <c r="C299" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="300" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B300" s="6"/>
+      <c r="C300" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="301" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B301" s="6"/>
+      <c r="C301" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="302" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B302" s="6"/>
+      <c r="C302" s="2" t="s">
+        <v>486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mid-progress update: methods and tools list
</commit_message>
<xml_diff>
--- a/data/data-sources.xlsx
+++ b/data/data-sources.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="900" windowWidth="18345" windowHeight="4095"/>
+    <workbookView xWindow="510" yWindow="900" windowWidth="11355" windowHeight="4095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data sources" sheetId="1" r:id="rId1"/>
+    <sheet name="methods, tools and practices" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="767">
   <si>
     <t>http://www.gbif.org/</t>
   </si>
@@ -1565,6 +1567,765 @@
   </si>
   <si>
     <t>tools and resources for assessing social impact</t>
+  </si>
+  <si>
+    <t>Environmental Capital Group</t>
+  </si>
+  <si>
+    <t>OECD DAC Network on Development Evaluation</t>
+  </si>
+  <si>
+    <t>The World Bank</t>
+  </si>
+  <si>
+    <t>Innovation Network</t>
+  </si>
+  <si>
+    <t>The William &amp; Flora Hewlett Foundation</t>
+  </si>
+  <si>
+    <t>European Foundation for Quality Management</t>
+  </si>
+  <si>
+    <t>William and Flora Hewlett Foundation</t>
+  </si>
+  <si>
+    <t>Doris Duke Charitable Foundation</t>
+  </si>
+  <si>
+    <t>TransFair USA</t>
+  </si>
+  <si>
+    <t>James Irvine Foundation</t>
+  </si>
+  <si>
+    <t>Robert Wood Johnson Foundation</t>
+  </si>
+  <si>
+    <t>Foundations of Success</t>
+  </si>
+  <si>
+    <t>Centers for Disease Control &amp; Prevention</t>
+  </si>
+  <si>
+    <t>San Francisco Department on the Status of Women, Calvert Group, Ltd., Verité</t>
+  </si>
+  <si>
+    <t>RAND Corporation, University of South Carolina, Centers for Disease Control and Prevention</t>
+  </si>
+  <si>
+    <t>Planet Rating</t>
+  </si>
+  <si>
+    <t>GiveWell</t>
+  </si>
+  <si>
+    <t>B Lab</t>
+  </si>
+  <si>
+    <t>GreatNonprofits</t>
+  </si>
+  <si>
+    <t>Global Reporting Initiative</t>
+  </si>
+  <si>
+    <t>GuideStar</t>
+  </si>
+  <si>
+    <t>Humanitarian Accountability Partnership (HAP) International</t>
+  </si>
+  <si>
+    <t>HIP Investor, Inc.</t>
+  </si>
+  <si>
+    <t>The Global Impact Investing Network (GIIN)</t>
+  </si>
+  <si>
+    <t>U.S. Department of Education</t>
+  </si>
+  <si>
+    <t>KaBOOM!</t>
+  </si>
+  <si>
+    <t>Annie E. Casey Foundation, Innovation Network</t>
+  </si>
+  <si>
+    <t>Corporate Citizenship</t>
+  </si>
+  <si>
+    <t>U.S. Green Building Council</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/browse.php</t>
+  </si>
+  <si>
+    <t>Grantmakers for Effective Organizations</t>
+  </si>
+  <si>
+    <t>Mango, Concern Worldwide</t>
+  </si>
+  <si>
+    <t>New Economics Foundation</t>
+  </si>
+  <si>
+    <t>Women's Funding Network</t>
+  </si>
+  <si>
+    <t>Urban Institute</t>
+  </si>
+  <si>
+    <t>World Business Council for Sustainable Development</t>
+  </si>
+  <si>
+    <t>Investing for Good</t>
+  </si>
+  <si>
+    <t>True Impact</t>
+  </si>
+  <si>
+    <t>USC Program for Environmental and Regional Equity</t>
+  </si>
+  <si>
+    <t>CIVICUS World Alliance for Citizen Participation</t>
+  </si>
+  <si>
+    <t>Microcredit Summit Campaign</t>
+  </si>
+  <si>
+    <t>Nurse-Family Partnership (NFP)</t>
+  </si>
+  <si>
+    <t>Marguerite Casey Foundation</t>
+  </si>
+  <si>
+    <t>McKinsey &amp; Company, Venture Philanthropy Partners</t>
+  </si>
+  <si>
+    <t>International Development Research Centre</t>
+  </si>
+  <si>
+    <t>Organizational Research Services</t>
+  </si>
+  <si>
+    <t>Center for What Works, Urban Institute</t>
+  </si>
+  <si>
+    <t>Pacific Community Ventures</t>
+  </si>
+  <si>
+    <t>Jill Blair, Fay Twersky</t>
+  </si>
+  <si>
+    <t>Urban Institute, ChildTrends, Social Solutions</t>
+  </si>
+  <si>
+    <t>Skyline Public Works</t>
+  </si>
+  <si>
+    <t>Charities Evaluation Services</t>
+  </si>
+  <si>
+    <t>Plan International</t>
+  </si>
+  <si>
+    <t>Grameen Foundation</t>
+  </si>
+  <si>
+    <t>Center for Effective Philanthropy, Grants Managers Network</t>
+  </si>
+  <si>
+    <t>MicroFinance Centre</t>
+  </si>
+  <si>
+    <t>Global Economy &amp; Development at Brookings, Center for Global Development</t>
+  </si>
+  <si>
+    <t>Roca</t>
+  </si>
+  <si>
+    <t>SEEP</t>
+  </si>
+  <si>
+    <t>ACCION</t>
+  </si>
+  <si>
+    <t>Social Audit Network</t>
+  </si>
+  <si>
+    <t>Social Evaluator</t>
+  </si>
+  <si>
+    <t>Rockefeller Foundation, Goldman Sachs Foundation</t>
+  </si>
+  <si>
+    <t>Global Social Venture Competition</t>
+  </si>
+  <si>
+    <t>SEEDA, European Social Fund, University of Brighton, Focus Work, SEL, The Cubist</t>
+  </si>
+  <si>
+    <t>Cúnamh ICT</t>
+  </si>
+  <si>
+    <t>Hunter Consulting LLC</t>
+  </si>
+  <si>
+    <t>REDF</t>
+  </si>
+  <si>
+    <t>USAID</t>
+  </si>
+  <si>
+    <t>CERISE</t>
+  </si>
+  <si>
+    <t>M-CRIL</t>
+  </si>
+  <si>
+    <t>MicroFinanza Rating</t>
+  </si>
+  <si>
+    <t>Root Capital</t>
+  </si>
+  <si>
+    <t>Nexus</t>
+  </si>
+  <si>
+    <t>The SROI Network</t>
+  </si>
+  <si>
+    <t>ESROIN members and others</t>
+  </si>
+  <si>
+    <t>Santa Clara University GSBI™</t>
+  </si>
+  <si>
+    <t>SVT Group</t>
+  </si>
+  <si>
+    <t>Standards for Excellence Institute</t>
+  </si>
+  <si>
+    <t>Margaret Sanger Center International, Planned Parenthood</t>
+  </si>
+  <si>
+    <t>NeighborWorks America</t>
+  </si>
+  <si>
+    <t>Triple Bottom Line Collaborative</t>
+  </si>
+  <si>
+    <t>Scottish Council for Voluntary Organisations</t>
+  </si>
+  <si>
+    <t>Grantmakers for Effective Organizations, La Piana Consulting</t>
+  </si>
+  <si>
+    <t>FINCA</t>
+  </si>
+  <si>
+    <t>Harvard Institute for International Development, Women in Development office of USAID</t>
+  </si>
+  <si>
+    <t>Triangle Consulting</t>
+  </si>
+  <si>
+    <t>FSG, Hallie Preskill &amp; Rosalie T. Torres</t>
+  </si>
+  <si>
+    <t>Impact Investment Shujog</t>
+  </si>
+  <si>
+    <t>Carol Weiss, et al.</t>
+  </si>
+  <si>
+    <t>Trucost PLC</t>
+  </si>
+  <si>
+    <t>Idealware</t>
+  </si>
+  <si>
+    <t>Institute for Volunteering Research</t>
+  </si>
+  <si>
+    <t>Wallace Foundation</t>
+  </si>
+  <si>
+    <t>Sara Hlupekile Longwe</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=10</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=143</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=5</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=98</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=151</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=30</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=38</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=1</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=109</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=11</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=33</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=196</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=12</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=13</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=117</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=200</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=14</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=86</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=15</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=97</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=45</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=73</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=46</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=184</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=144</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=188</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=16</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=128</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=191</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=82</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=28</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=160</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=129</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=31</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=32</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=50</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=47</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=93</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=169</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=53</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=83</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=78</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=203</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=183</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=40</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=199</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=55</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=63</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=125</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=56</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=100</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=133</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=74</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=198</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=58</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=150</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=54</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=134</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=79</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=107</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=60</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=35</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=156</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=158</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=104</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=62</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=110</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=49</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=70</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=64</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=71</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=162</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=72</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=108</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=6</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=17</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=137</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=81</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=18</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=19</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=185</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=140</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=68</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=84</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=20</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=87</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=69</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=95</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=75</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=168</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=139</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=61</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=7</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=161</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=21</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=172</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=194</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=192</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=92</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=187</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=174</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=89</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=41</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=163</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=42</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=76</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=186</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=142</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=176</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=101</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=138</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=102</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=80</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=178</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=189</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=22</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=23</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=24</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=99</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=132</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=44</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=193</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=145</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=103</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=67</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=146</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=147</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=148</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=170</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=96</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=4</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=90</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=155</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=164</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=120</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=121</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=122</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=123</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=124</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=2</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=165</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=167</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=111</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=66</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=119</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=182</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=126</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=106</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=141</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=52</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=88</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=91</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=112</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=181</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=25</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=105</t>
+  </si>
+  <si>
+    <t>http://trasi.foundationcenter.org/record.php?SN=131</t>
   </si>
 </sst>
 </file>
@@ -1591,7 +2352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1610,6 +2371,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1623,7 +2390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1641,6 +2408,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1949,10 +2719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U302"/>
+  <dimension ref="B1:U108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109:XFD307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1960,7 +2730,7 @@
     <col min="1" max="1" width="6" style="2" customWidth="1"/>
     <col min="2" max="2" width="28.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="37.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="60.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" style="2" hidden="1" customWidth="1"/>
     <col min="5" max="21" width="17.28515625" style="2" customWidth="1"/>
     <col min="22" max="16384" width="14.42578125" style="2"/>
   </cols>
@@ -3405,7 +4175,7 @@
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
     </row>
-    <row r="54" spans="2:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:21" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>133</v>
       </c>
@@ -4815,1534 +5585,2739 @@
         <v>513</v>
       </c>
     </row>
-    <row r="110" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G199"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B160" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B168" sqref="B168"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>630</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
+        <v>639</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
+        <v>640</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
+        <v>647</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="6" t="s">
+        <v>659</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="6" t="s">
+        <v>660</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="6" t="s">
+        <v>661</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="6" t="s">
+        <v>662</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="s">
+        <v>664</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="6" t="s">
+        <v>666</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="6" t="s">
+        <v>667</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="6" t="s">
+        <v>668</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="6" t="s">
+        <v>670</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="6" t="s">
+        <v>672</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="6" t="s">
+        <v>674</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="6" t="s">
+        <v>675</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="6" t="s">
+        <v>676</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="6" t="s">
+        <v>677</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="6" t="s">
+        <v>678</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="6" t="s">
+        <v>679</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="6" t="s">
+        <v>680</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="6" t="s">
+        <v>681</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="6" t="s">
+        <v>682</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="6" t="s">
+        <v>683</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="6" t="s">
+        <v>684</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="6" t="s">
+        <v>685</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="6" t="s">
+        <v>686</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="6" t="s">
+        <v>687</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="6" t="s">
+        <v>688</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="6" t="s">
+        <v>689</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="6" t="s">
+        <v>690</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="6" t="s">
+        <v>691</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="6" t="s">
+        <v>692</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="6" t="s">
+        <v>693</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="6" t="s">
+        <v>694</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="6" t="s">
+        <v>695</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="6" t="s">
+        <v>696</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="6" t="s">
+        <v>697</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="6" t="s">
+        <v>698</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="6" t="s">
+        <v>699</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="6" t="s">
+        <v>700</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="6" t="s">
+        <v>701</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="6" t="s">
+        <v>702</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="6" t="s">
+        <v>703</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="6" t="s">
+        <v>704</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="6" t="s">
+        <v>705</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="6" t="s">
+        <v>706</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="6" t="s">
-        <v>258</v>
+        <v>708</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>257</v>
+        <v>402</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>259</v>
+        <v>402</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="111" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="6" t="s">
-        <v>262</v>
+        <v>709</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>261</v>
+        <v>403</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>263</v>
+        <v>554</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="112" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="6" t="s">
-        <v>267</v>
+        <v>710</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>264</v>
+        <v>404</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>265</v>
+        <v>516</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="6" t="s">
-        <v>269</v>
+        <v>711</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>268</v>
+        <v>405</v>
       </c>
       <c r="E113" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E114" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="F113" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="114" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="F114" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="6" t="s">
+        <v>713</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="115" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="116" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="6" t="s">
-        <v>280</v>
+        <v>714</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>278</v>
+        <v>408</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="117" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="6" t="s">
-        <v>283</v>
+        <v>715</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>281</v>
+        <v>409</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>282</v>
+        <v>517</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="6"/>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="6" t="s">
+        <v>716</v>
+      </c>
       <c r="C118" s="2" t="s">
-        <v>284</v>
+        <v>410</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>273</v>
+        <v>557</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="119" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="6"/>
+    <row r="119" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="6" t="s">
+        <v>717</v>
+      </c>
       <c r="C119" s="2" t="s">
-        <v>285</v>
+        <v>411</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>286</v>
+        <v>558</v>
       </c>
       <c r="F119" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="120" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="6"/>
+    <row r="120" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="6" t="s">
+        <v>718</v>
+      </c>
       <c r="C120" s="2" t="s">
-        <v>287</v>
+        <v>412</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>288</v>
+        <v>559</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="121" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="6"/>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="6" t="s">
+        <v>719</v>
+      </c>
       <c r="C121" s="2" t="s">
-        <v>289</v>
+        <v>413</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>290</v>
+        <v>560</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="122" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="6"/>
+    <row r="122" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="6" t="s">
+        <v>720</v>
+      </c>
       <c r="C122" s="2" t="s">
-        <v>291</v>
+        <v>414</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>292</v>
+        <v>561</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="123" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="6"/>
+    <row r="123" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="6" t="s">
+        <v>721</v>
+      </c>
       <c r="C123" s="2" t="s">
-        <v>293</v>
+        <v>415</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>294</v>
+        <v>562</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="G123" s="2" t="s">
+    </row>
+    <row r="124" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G130" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="124" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="6"/>
-      <c r="C124" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="125" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="6"/>
-      <c r="C125" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="126" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="6"/>
-      <c r="C126" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="6"/>
-      <c r="C127" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="128" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="6"/>
-      <c r="C128" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="F128" s="2" t="s">
+    <row r="131" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="6" t="s">
+        <v>729</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="F131" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="129" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="6"/>
-      <c r="C129" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="130" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="6"/>
-      <c r="C130" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="E130" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F130" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="131" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="6"/>
-      <c r="C131" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="E131" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="132" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="6"/>
+    <row r="132" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="6" t="s">
+        <v>730</v>
+      </c>
       <c r="C132" s="2" t="s">
-        <v>318</v>
+        <v>424</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>487</v>
+        <v>566</v>
       </c>
       <c r="F132" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="F135" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="133" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="6"/>
-      <c r="C133" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="134" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="6"/>
-      <c r="C134" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="135" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="6"/>
-      <c r="C135" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="136" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="6"/>
+    <row r="136" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="6" t="s">
+        <v>734</v>
+      </c>
       <c r="C136" s="2" t="s">
-        <v>322</v>
+        <v>428</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>273</v>
+        <v>568</v>
       </c>
       <c r="F136" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="F137" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="137" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="6"/>
-      <c r="C137" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E137" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="138" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="6"/>
+    <row r="138" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="6" t="s">
+        <v>736</v>
+      </c>
       <c r="C138" s="2" t="s">
-        <v>324</v>
+        <v>430</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="139" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="6"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="6" t="s">
+        <v>737</v>
+      </c>
       <c r="C139" s="2" t="s">
-        <v>325</v>
+        <v>431</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="F139" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="140" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="6"/>
+    <row r="140" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="6" t="s">
+        <v>738</v>
+      </c>
       <c r="C140" s="2" t="s">
-        <v>326</v>
+        <v>432</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>493</v>
+        <v>569</v>
       </c>
       <c r="F140" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="6" t="s">
+        <v>739</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="6" t="s">
+        <v>740</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="6" t="s">
+        <v>741</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="6" t="s">
+        <v>742</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="145" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="6" t="s">
+        <v>743</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="146" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="149" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="150" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B150" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="151" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="152" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="153" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="154" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B154" s="6" t="s">
+        <v>752</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="F154" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="141" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="6"/>
-      <c r="C141" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E141" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="142" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="6"/>
-      <c r="C142" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E142" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="F142" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="143" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="6"/>
-      <c r="C143" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="144" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="6"/>
-      <c r="C144" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E144" s="2" t="s">
+    <row r="155" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="6" t="s">
+        <v>753</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="156" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="157" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="6" t="s">
+        <v>755</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="158" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="6" t="s">
+        <v>756</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="159" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="6" t="s">
+        <v>757</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="160" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="6" t="s">
+        <v>758</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="6" t="s">
+        <v>759</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="6" t="s">
+        <v>760</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G162" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="6" t="s">
+        <v>761</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G163" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="6" t="s">
+        <v>762</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="6" t="s">
+        <v>763</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="F165" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="6" t="s">
+        <v>764</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E166" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F144" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="145" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="6"/>
-      <c r="C145" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="E145" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="F145" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="146" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="6"/>
-      <c r="C146" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="E146" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="F146" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="147" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="6"/>
-      <c r="C147" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="F147" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="148" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="6"/>
-      <c r="C148" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="E148" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="F148" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="G148" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="149" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="6"/>
-      <c r="C149" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="E149" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="F149" s="2" t="s">
+      <c r="F166" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="167" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="6" t="s">
+        <v>765</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="6" t="s">
+        <v>766</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="F168" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="150" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="6"/>
-      <c r="C150" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="E150" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="F150" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="151" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="6"/>
-      <c r="C151" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F151" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="152" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="6"/>
-      <c r="C152" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E152" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F152" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="153" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="6"/>
-      <c r="C153" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="F153" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="154" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="6"/>
-      <c r="C154" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="E154" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="F154" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="G154" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="155" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="6"/>
-      <c r="C155" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="E155" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="F155" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="156" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="6"/>
-      <c r="C156" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="E156" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="F156" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="157" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="6"/>
-      <c r="C157" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="E157" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="F157" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="158" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="6"/>
-      <c r="C158" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="F158" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="159" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="6"/>
-      <c r="C159" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="E159" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="F159" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="160" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="6"/>
-      <c r="C160" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="F160" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="161" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="6"/>
-      <c r="C161" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="E161" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="F161" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="162" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="6"/>
-      <c r="C162" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="F162" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="163" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="6"/>
-      <c r="C163" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="E163" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="F163" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="164" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="6"/>
-      <c r="C164" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="E164" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="F164" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="165" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B165" s="6"/>
-      <c r="C165" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="E165" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="F165" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="G165" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="166" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="6"/>
-      <c r="C166" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="F166" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="167" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="6"/>
-      <c r="C167" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="168" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B168" s="6"/>
-      <c r="C168" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="169" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
       <c r="C169" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="170" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="F169" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
       <c r="C170" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="171" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="F170" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="171" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="6"/>
       <c r="C171" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="172" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="F171" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="6"/>
       <c r="C172" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="173" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F172" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="6"/>
       <c r="C173" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="174" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F173" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="6"/>
       <c r="C174" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="175" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="F174" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G174" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="6"/>
       <c r="C175" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="176" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="F175" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="176" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="6"/>
       <c r="C176" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="177" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="F176" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="6"/>
       <c r="C177" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="178" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="F177" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="178" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="6"/>
       <c r="C178" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="179" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F178" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="6"/>
       <c r="C179" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="180" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="F179" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="6"/>
       <c r="C180" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="181" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="F180" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G180" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="181" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="6"/>
       <c r="C181" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="182" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="F181" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="182" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="6"/>
       <c r="C182" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="183" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="F182" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="183" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="6"/>
       <c r="C183" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="184" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="F183" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="184" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="6"/>
       <c r="C184" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="185" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>474</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="F184" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="185" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="6"/>
       <c r="C185" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="186" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>475</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="F185" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="186" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" s="6"/>
       <c r="C186" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="187" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="187" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="6"/>
       <c r="C187" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="188" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+      <c r="E187" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="188" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
       <c r="C188" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="189" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="F188" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="189" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="6"/>
       <c r="C189" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="190" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="190" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="6"/>
       <c r="C190" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="191" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="191" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="6"/>
       <c r="C191" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="192" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F191" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="192" spans="2:7" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="6"/>
       <c r="C192" s="2" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="193" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>482</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="F192" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="193" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="6"/>
       <c r="C193" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="194" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+      <c r="E193" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="F193" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="194" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="6"/>
       <c r="C194" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="195" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>484</v>
+      </c>
+      <c r="E194" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F194" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="195" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="6"/>
       <c r="C195" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="196" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+      <c r="E195" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="F195" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="196" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="6"/>
       <c r="C196" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="197" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="6"/>
-      <c r="C197" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="198" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="6"/>
-      <c r="C198" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="199" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B199" s="6"/>
-      <c r="C199" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="200" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="6"/>
-      <c r="C200" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="201" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B201" s="6"/>
-      <c r="C201" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="202" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="6"/>
-      <c r="C202" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="203" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="6"/>
-      <c r="C203" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="204" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="6"/>
-      <c r="C204" s="2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="205" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="6"/>
-      <c r="C205" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="206" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="6"/>
-      <c r="C206" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="207" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="6"/>
-      <c r="C207" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="208" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B208" s="6"/>
-      <c r="C208" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="209" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B209" s="6"/>
-      <c r="C209" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="210" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B210" s="6"/>
-      <c r="C210" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="211" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B211" s="6"/>
-      <c r="C211" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="212" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B212" s="6"/>
-      <c r="C212" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="213" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B213" s="6"/>
-      <c r="C213" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="214" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B214" s="6"/>
-      <c r="C214" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="215" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B215" s="6"/>
-      <c r="C215" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="216" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B216" s="6"/>
-      <c r="C216" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="217" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B217" s="6"/>
-      <c r="C217" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="218" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B218" s="6"/>
-      <c r="C218" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="219" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B219" s="6"/>
-      <c r="C219" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="220" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B220" s="6"/>
-      <c r="C220" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="221" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B221" s="6"/>
-      <c r="C221" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="222" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B222" s="6"/>
-      <c r="C222" s="2" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="223" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B223" s="6"/>
-      <c r="C223" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="224" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="6"/>
-      <c r="C224" s="2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="225" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B225" s="6"/>
-      <c r="C225" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="226" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B226" s="6"/>
-      <c r="C226" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="227" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B227" s="6"/>
-      <c r="C227" s="2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="228" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B228" s="6"/>
-      <c r="C228" s="2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="229" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B229" s="6"/>
-      <c r="C229" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="230" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B230" s="6"/>
-      <c r="C230" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="231" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B231" s="6"/>
-      <c r="C231" s="2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="232" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B232" s="6"/>
-      <c r="C232" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="233" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B233" s="6"/>
-      <c r="C233" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="234" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B234" s="6"/>
-      <c r="C234" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="235" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B235" s="6"/>
-      <c r="C235" s="2" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="236" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B236" s="6"/>
-      <c r="C236" s="2" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="237" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B237" s="6"/>
-      <c r="C237" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="238" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B238" s="6"/>
-      <c r="C238" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="239" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B239" s="6"/>
-      <c r="C239" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="240" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B240" s="6"/>
-      <c r="C240" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="241" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B241" s="6"/>
-      <c r="C241" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="242" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B242" s="6"/>
-      <c r="C242" s="2" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="243" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B243" s="6"/>
-      <c r="C243" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="244" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B244" s="6"/>
-      <c r="C244" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="245" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B245" s="6"/>
-      <c r="C245" s="2" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="246" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B246" s="6"/>
-      <c r="C246" s="2" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="247" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B247" s="6"/>
-      <c r="C247" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="248" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B248" s="6"/>
-      <c r="C248" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="249" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B249" s="6"/>
-      <c r="C249" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="250" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B250" s="6"/>
-      <c r="C250" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="251" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B251" s="6"/>
-      <c r="C251" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="252" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B252" s="6"/>
-      <c r="C252" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="253" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B253" s="6"/>
-      <c r="C253" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="254" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B254" s="6"/>
-      <c r="C254" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="255" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B255" s="6"/>
-      <c r="C255" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="256" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B256" s="6"/>
-      <c r="C256" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="257" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B257" s="6"/>
-      <c r="C257" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="258" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B258" s="6"/>
-      <c r="C258" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="259" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B259" s="6"/>
-      <c r="C259" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="260" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B260" s="6"/>
-      <c r="C260" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="261" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B261" s="6"/>
-      <c r="C261" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="262" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B262" s="6"/>
-      <c r="C262" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="263" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B263" s="6"/>
-      <c r="C263" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="264" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B264" s="6"/>
-      <c r="C264" s="2" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="265" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B265" s="6"/>
-      <c r="C265" s="2" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="266" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B266" s="6"/>
-      <c r="C266" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="267" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B267" s="6"/>
-      <c r="C267" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="268" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B268" s="6"/>
-      <c r="C268" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="269" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B269" s="6"/>
-      <c r="C269" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="270" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B270" s="6"/>
-      <c r="C270" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="271" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B271" s="6"/>
-      <c r="C271" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="272" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B272" s="6"/>
-      <c r="C272" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="273" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B273" s="6"/>
-      <c r="C273" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="274" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B274" s="6"/>
-      <c r="C274" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="275" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B275" s="6"/>
-      <c r="C275" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="276" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B276" s="6"/>
-      <c r="C276" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="277" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B277" s="6"/>
-      <c r="C277" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="278" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B278" s="6"/>
-      <c r="C278" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="279" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B279" s="6"/>
-      <c r="C279" s="2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="280" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B280" s="6"/>
-      <c r="C280" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="281" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B281" s="6"/>
-      <c r="C281" s="2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="282" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B282" s="6"/>
-      <c r="C282" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="283" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B283" s="6"/>
-      <c r="C283" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="284" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B284" s="6"/>
-      <c r="C284" s="2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="285" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B285" s="6"/>
-      <c r="C285" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="286" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B286" s="6"/>
-      <c r="C286" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="287" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B287" s="6"/>
-      <c r="C287" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="288" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B288" s="6"/>
-      <c r="C288" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="289" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B289" s="6"/>
-      <c r="C289" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="290" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B290" s="6"/>
-      <c r="C290" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="291" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B291" s="6"/>
-      <c r="C291" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="292" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B292" s="6"/>
-      <c r="C292" s="2" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="293" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B293" s="6"/>
-      <c r="C293" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="294" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B294" s="6"/>
-      <c r="C294" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="295" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B295" s="6"/>
-      <c r="C295" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="296" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B296" s="6"/>
-      <c r="C296" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="297" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B297" s="6"/>
-      <c r="C297" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="298" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B298" s="6"/>
-      <c r="C298" s="2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="299" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B299" s="6"/>
-      <c r="C299" s="2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="300" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B300" s="6"/>
-      <c r="C300" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="301" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B301" s="6"/>
-      <c r="C301" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="302" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B302" s="6"/>
-      <c r="C302" s="2" t="s">
         <v>486</v>
       </c>
-    </row>
+      <c r="E196" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="F196" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="197" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="2:6" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>